<commit_message>
Fix preposition for Harrow
</commit_message>
<xml_diff>
--- a/data/postcodes/input/postcode-area-names.xlsx
+++ b/data/postcodes/input/postcode-area-names.xlsx
@@ -1139,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1618,7 +1618,7 @@
         <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>